<commit_message>
3/13 python tensorflow test
</commit_message>
<xml_diff>
--- a/section12/helloworld.xlsx
+++ b/section12/helloworld.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -381,681 +381,691 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>난민</t>
+          <t>대표</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>한국</t>
+          <t>기자</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>서울</t>
+          <t>한국</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>기자</t>
+          <t>대해</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>대표</t>
+          <t>기술</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>대해</t>
+          <t>지역</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>때문</t>
+          <t>사업</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>현대차</t>
+          <t>대한</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>지난해</t>
+          <t>국회</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>신청</t>
+          <t>금지</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>의원</t>
+          <t>무단</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>경우</t>
+          <t>북한</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>대한</t>
+          <t>원내대표</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>통해</t>
+          <t>조사</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>이번</t>
+          <t>지난해</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>민주당</t>
+          <t>위해</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>원내대표</t>
+          <t>서울</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>계획</t>
+          <t>배포</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>사업</t>
+          <t>민주당</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>위해</t>
+          <t>의원</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>대통령</t>
+          <t>문화</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>문제</t>
+          <t>통해</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>관련</t>
+          <t>총리</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>주장</t>
+          <t>때문</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>기술</t>
+          <t>서비스</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>금지</t>
+          <t>처리</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>전망</t>
+          <t>계획</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>배포</t>
+          <t>관련</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>서울시</t>
+          <t>확대</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>무단</t>
+          <t>중단</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>정부</t>
+          <t>미국</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>북한</t>
+          <t>이후</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>미국</t>
+          <t>시장</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>합의</t>
+          <t>관리</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>이후</t>
+          <t>사람</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>지원</t>
+          <t>정부</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>엘리엇</t>
+          <t>합의</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>업체</t>
+          <t>라며</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>담낭</t>
+          <t>발언</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>국가</t>
+          <t>문제</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>지난</t>
+          <t>정준영</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>미세먼지</t>
+          <t>사용</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>최근</t>
+          <t>모델</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>라며</t>
+          <t>지난</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>인도</t>
+          <t>뉴스</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>보잉</t>
+          <t>이번</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>위원장</t>
+          <t>개발</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>후보</t>
+          <t>가장</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>관계자</t>
+          <t>고시원</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>현재</t>
+          <t>미세먼지</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>조사</t>
+          <t>내용</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>배당</t>
+          <t>위원회</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>비소</t>
+          <t>진행</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>모두</t>
+          <t>위원장</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>수준</t>
+          <t>국민</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>박스</t>
+          <t>이상</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>정책</t>
+          <t>설명</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>경제</t>
+          <t>아베</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>시장</t>
+          <t>개정안</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>소송</t>
+          <t>개선</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>제안</t>
+          <t>시간</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>여성</t>
+          <t>운항</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>사외이사</t>
+          <t>연설</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>기온</t>
+          <t>르노</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>영하</t>
+          <t>올해</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>발언</t>
+          <t>국가</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>총장</t>
+          <t>면서</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>대변인</t>
+          <t>대통령</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>증가</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>